<commit_message>
perf(controller, xlspython): do a file save not at every sheet but only when all sheets are modified to gain time when running
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_extract_column.xlsx
+++ b/fichiers_xls/test_extract_column.xlsx
@@ -11,7 +11,6 @@
     <sheet name="22303499" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="22302237" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="22304999" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="gather_2" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
@@ -3188,555 +3187,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D46"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>22300896</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>22303499</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>22302237</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>22304999</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>4479</v>
-      </c>
-      <c r="B2" t="n">
-        <v>9003</v>
-      </c>
-      <c r="C2" t="n">
-        <v>4574</v>
-      </c>
-      <c r="D2" t="n">
-        <v>2480</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>8814</v>
-      </c>
-      <c r="B3" t="n">
-        <v>11301</v>
-      </c>
-      <c r="C3" t="n">
-        <v>7308</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2447</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3862</v>
-      </c>
-      <c r="B4" t="n">
-        <v>4477</v>
-      </c>
-      <c r="C4" t="n">
-        <v>4518</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1734</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>11797</v>
-      </c>
-      <c r="B5" t="n">
-        <v>4313</v>
-      </c>
-      <c r="C5" t="n">
-        <v>5067</v>
-      </c>
-      <c r="D5" t="n">
-        <v>2631</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>2322</v>
-      </c>
-      <c r="B6" t="n">
-        <v>10197</v>
-      </c>
-      <c r="C6" t="n">
-        <v>7838</v>
-      </c>
-      <c r="D6" t="n">
-        <v>3278</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6286</v>
-      </c>
-      <c r="B7" t="n">
-        <v>16577</v>
-      </c>
-      <c r="C7" t="n">
-        <v>11263</v>
-      </c>
-      <c r="D7" t="n">
-        <v>2434</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>15306</v>
-      </c>
-      <c r="B8" t="n">
-        <v>4209</v>
-      </c>
-      <c r="C8" t="n">
-        <v>10119</v>
-      </c>
-      <c r="D8" t="n">
-        <v>2366</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>14358</v>
-      </c>
-      <c r="B9" t="n">
-        <v>5398</v>
-      </c>
-      <c r="C9" t="n">
-        <v>6883</v>
-      </c>
-      <c r="D9" t="n">
-        <v>3310</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>3921</v>
-      </c>
-      <c r="B10" t="n">
-        <v>3195</v>
-      </c>
-      <c r="C10" t="n">
-        <v>9096</v>
-      </c>
-      <c r="D10" t="n">
-        <v>3737</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>11250</v>
-      </c>
-      <c r="B11" t="n">
-        <v>8510</v>
-      </c>
-      <c r="C11" t="n">
-        <v>10865</v>
-      </c>
-      <c r="D11" t="n">
-        <v>3467</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>10283</v>
-      </c>
-      <c r="B12" t="n">
-        <v>3644</v>
-      </c>
-      <c r="C12" t="n">
-        <v>8195</v>
-      </c>
-      <c r="D12" t="n">
-        <v>3816</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>22260</v>
-      </c>
-      <c r="B13" t="n">
-        <v>23079</v>
-      </c>
-      <c r="C13" t="n">
-        <v>2766</v>
-      </c>
-      <c r="D13" t="n">
-        <v>3188</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>4145</v>
-      </c>
-      <c r="B14" t="n">
-        <v>13445</v>
-      </c>
-      <c r="C14" t="n">
-        <v>6754</v>
-      </c>
-      <c r="D14" t="n">
-        <v>6292</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>7644</v>
-      </c>
-      <c r="B15" t="n">
-        <v>5829</v>
-      </c>
-      <c r="C15" t="n">
-        <v>39419</v>
-      </c>
-      <c r="D15" t="n">
-        <v>1978</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>6710</v>
-      </c>
-      <c r="B16" t="n">
-        <v>4278</v>
-      </c>
-      <c r="C16" t="n">
-        <v>13531</v>
-      </c>
-      <c r="D16" t="n">
-        <v>2368</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>11768</v>
-      </c>
-      <c r="B17" t="n">
-        <v>2229</v>
-      </c>
-      <c r="C17" t="n">
-        <v>10292</v>
-      </c>
-      <c r="D17" t="n">
-        <v>2212</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>1711</v>
-      </c>
-      <c r="B18" t="n">
-        <v>4157</v>
-      </c>
-      <c r="C18" t="n">
-        <v>18927</v>
-      </c>
-      <c r="D18" t="n">
-        <v>1501</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>2597</v>
-      </c>
-      <c r="B19" t="n">
-        <v>4814</v>
-      </c>
-      <c r="C19" t="n">
-        <v>10683</v>
-      </c>
-      <c r="D19" t="n">
-        <v>1953</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>1346</v>
-      </c>
-      <c r="B20" t="n">
-        <v>17163</v>
-      </c>
-      <c r="C20" t="n">
-        <v>23540</v>
-      </c>
-      <c r="D20" t="n">
-        <v>1669</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>9118</v>
-      </c>
-      <c r="B21" t="n">
-        <v>4063</v>
-      </c>
-      <c r="C21" t="n">
-        <v>1552</v>
-      </c>
-      <c r="D21" t="n">
-        <v>5404</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>2172</v>
-      </c>
-      <c r="B22" t="n">
-        <v>7476</v>
-      </c>
-      <c r="C22" t="n">
-        <v>20740</v>
-      </c>
-      <c r="D22" t="n">
-        <v>4359</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>6452</v>
-      </c>
-      <c r="B23" t="n">
-        <v>2497</v>
-      </c>
-      <c r="C23" t="n">
-        <v>21109</v>
-      </c>
-      <c r="D23" t="n">
-        <v>1609</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>1287</v>
-      </c>
-      <c r="B24" t="n">
-        <v>5812</v>
-      </c>
-      <c r="C24" t="n">
-        <v>16533</v>
-      </c>
-      <c r="D24" t="n">
-        <v>2729</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>1881</v>
-      </c>
-      <c r="B25" t="n">
-        <v>6496</v>
-      </c>
-      <c r="C25" t="n">
-        <v>12421</v>
-      </c>
-      <c r="D25" t="n">
-        <v>1928</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>2070</v>
-      </c>
-      <c r="B26" t="n">
-        <v>11044</v>
-      </c>
-      <c r="C26" t="n">
-        <v>4383</v>
-      </c>
-      <c r="D26" t="n">
-        <v>2817</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>7729</v>
-      </c>
-      <c r="B27" t="n">
-        <v>8330</v>
-      </c>
-      <c r="C27" t="n">
-        <v>16564</v>
-      </c>
-      <c r="D27" t="n">
-        <v>2308</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>2572</v>
-      </c>
-      <c r="B28" t="n">
-        <v>8561</v>
-      </c>
-      <c r="C28" t="n">
-        <v>8168</v>
-      </c>
-      <c r="D28" t="n">
-        <v>2359</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>9326</v>
-      </c>
-      <c r="B29" t="n">
-        <v>6693</v>
-      </c>
-      <c r="C29" t="n">
-        <v>15257</v>
-      </c>
-      <c r="D29" t="n">
-        <v>6204</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>8775</v>
-      </c>
-      <c r="B30" t="n">
-        <v>3078</v>
-      </c>
-      <c r="C30" t="n">
-        <v>15205</v>
-      </c>
-      <c r="D30" t="n">
-        <v>2760</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>2023</v>
-      </c>
-      <c r="B31" t="n">
-        <v>3704</v>
-      </c>
-      <c r="C31" t="n">
-        <v>12914</v>
-      </c>
-      <c r="D31" t="n">
-        <v>3750</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>1395</v>
-      </c>
-      <c r="B32" t="n">
-        <v>4369</v>
-      </c>
-      <c r="C32" t="n">
-        <v>12461</v>
-      </c>
-      <c r="D32" t="n">
-        <v>1727</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>6754</v>
-      </c>
-      <c r="C33" t="n">
-        <v>1861</v>
-      </c>
-      <c r="D33" t="n">
-        <v>3303</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="C34" t="n">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="C35" t="n">
-        <v>3871</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="C36" t="n">
-        <v>3843</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="C37" t="n">
-        <v>1221</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="C38" t="n">
-        <v>2427</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="C39" t="n">
-        <v>1287</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="C40" t="n">
-        <v>2417</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="C41" t="n">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="C42" t="n">
-        <v>1806</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="C43" t="n">
-        <v>1126</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="C44" t="n">
-        <v>2731</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="C45" t="n">
-        <v>3166</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="C46" t="n">
-        <v>6253</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>